<commit_message>
Time series structural changes and github-pages
</commit_message>
<xml_diff>
--- a/Data/2023 kaskaskia woods.xlsx
+++ b/Data/2023 kaskaskia woods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacobfraser\source\repos\Kaskaskia_OG\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A65DB28-80DB-4A95-89BD-A2081A63C535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689F3A80-59A6-4A49-B02B-C8525E890FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" activeTab="1" xr2:uid="{24BDB0FC-F12F-4E7B-BBBB-81660EC46C29}"/>
+    <workbookView xWindow="-19200" yWindow="0" windowWidth="19200" windowHeight="21140" activeTab="1" xr2:uid="{24BDB0FC-F12F-4E7B-BBBB-81660EC46C29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5910" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5911" uniqueCount="92">
   <si>
     <t>Plot #</t>
   </si>
@@ -338,6 +338,9 @@
   <si>
     <t>Missing tags</t>
   </si>
+  <si>
+    <t>7318 Tag???</t>
+  </si>
 </sst>
 </file>
 
@@ -550,7 +553,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -44428,9 +44431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A16C5F1-0207-415E-AC5E-B7B9C5E97D6E}">
   <dimension ref="A1:O483"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14"/>
@@ -44525,7 +44528,9 @@
         <v>3</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -45086,8 +45091,8 @@
       <c r="B17" s="5">
         <v>5618</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>35</v>
+      <c r="C17" s="5">
+        <v>9117</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="4">
@@ -45116,7 +45121,9 @@
         <v>7.8</v>
       </c>
       <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="O17" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="4">
@@ -49482,7 +49489,7 @@
         <v>15</v>
       </c>
       <c r="G130" s="35" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H130" s="1" t="s">
         <v>30</v>
@@ -56311,7 +56318,7 @@
         <v>23.5</v>
       </c>
       <c r="G311" s="4" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="H311" s="9" t="s">
         <v>30</v>
@@ -58027,7 +58034,7 @@
         <v>10.02792</v>
       </c>
       <c r="G357" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H357" s="9" t="s">
         <v>30</v>

</xml_diff>